<commit_message>
Atualizando leitor de excel para ignorar # na tarefa e ignorar tarefas já lançadas.
</commit_message>
<xml_diff>
--- a/ModeloExcelLancaHora.xlsx
+++ b/ModeloExcelLancaHora.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.magalhaes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LancadorRedmine\LancadorDeHorasRedmine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC98CC6-264A-464E-A28B-D9ABDB9F9FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87738BC-B564-4435-B84E-7A772BD4F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4305" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{659911D1-6418-4B70-A1FE-BC88514A9016}"/>
+    <workbookView xWindow="-23148" yWindow="-2028" windowWidth="23256" windowHeight="12456" xr2:uid="{659911D1-6418-4B70-A1FE-BC88514A9016}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Data</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Lista das opções de atividades do redmine</t>
+  </si>
+  <si>
+    <t>Lançado</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -252,6 +255,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,12 +269,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,11 +603,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9863EC3C-FCA9-42C6-AF23-EF5F864BD7C0}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +621,7 @@
     <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -641,8 +643,11 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
@@ -651,7 +656,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3"/>
@@ -660,7 +665,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
@@ -669,7 +674,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
@@ -678,7 +683,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>
@@ -688,6 +693,11 @@
       <c r="G6" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{305599D3-6205-454A-ADCF-E15E097E741E}">
+      <formula1>"Pendente, Lançado"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -719,88 +729,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="5"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>